<commit_message>
write reproducibility instructions; update curated_standards.xlsx; create .gitignore so keys.py doesn't get committed to GitHub
</commit_message>
<xml_diff>
--- a/curated_standards.xlsx
+++ b/curated_standards.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34740" yWindow="1920" windowWidth="28080" windowHeight="18680" tabRatio="352"/>
+    <workbookView xWindow="-36860" yWindow="3520" windowWidth="27400" windowHeight="18020" tabRatio="352"/>
   </bookViews>
   <sheets>
     <sheet name="Curated_standards" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="113">
   <si>
     <t>Standard / tool</t>
   </si>
@@ -315,12 +315,6 @@
   </si>
   <si>
     <t>The rationale of PROV</t>
-  </si>
-  <si>
-    <t>SBML2Prism</t>
-  </si>
-  <si>
-    <t>PRISM 4.0: Verification of probabilistic real-time systems</t>
   </si>
   <si>
     <t>SciUnit</t>
@@ -378,7 +372,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -396,6 +390,20 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -415,8 +423,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -431,7 +443,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -796,12 +812,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1420" topLeftCell="A30" activePane="bottomLeft"/>
+      <pane ySplit="1420" topLeftCell="A31" activePane="bottomLeft"/>
       <selection sqref="A1:B1"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -876,7 +892,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>30</v>
@@ -912,7 +928,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>44</v>
@@ -948,7 +964,7 @@
         <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>53</v>
@@ -959,7 +975,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>57</v>
@@ -992,7 +1008,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>51</v>
@@ -1061,7 +1077,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -1072,10 +1088,10 @@
         <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -1094,10 +1110,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>5</v>
@@ -1108,7 +1124,7 @@
         <v>94</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>95</v>
@@ -1130,7 +1146,7 @@
         <v>66</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>67</v>
@@ -1152,7 +1168,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>34</v>
@@ -1163,7 +1179,7 @@
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>22</v>
@@ -1185,7 +1201,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>12</v>
@@ -1193,164 +1209,153 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="1" t="s">
+    <row r="39" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A38" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="28" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="28" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="42" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="42" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
incorporate data from "A blueprint for human whole-cell modeling", 2018; remove unused code, comments; remove shell script -- will replace with portable python code
</commit_message>
<xml_diff>
--- a/curated_standards.xlsx
+++ b/curated_standards.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36860" yWindow="3520" windowWidth="27400" windowHeight="18020" tabRatio="352"/>
+    <workbookView xWindow="-32260" yWindow="2040" windowWidth="23820" windowHeight="19560" tabRatio="352"/>
   </bookViews>
   <sheets>
     <sheet name="Curated_standards" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
   <si>
     <t>Standard / tool</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>Model data annotation tool</t>
-  </si>
-  <si>
-    <t>Rule-based modeling language</t>
   </si>
   <si>
     <t>Biochemical data standard</t>
@@ -814,10 +811,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1420" topLeftCell="A31" activePane="bottomLeft"/>
-      <selection sqref="A1:B1"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="1420" activePane="bottomLeft"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -923,12 +920,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>44</v>
@@ -1008,7 +1005,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>51</v>
@@ -1091,7 +1088,7 @@
         <v>103</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -1113,7 +1110,7 @@
         <v>101</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>5</v>
@@ -1124,7 +1121,7 @@
         <v>94</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>95</v>
@@ -1242,7 +1239,7 @@
     </row>
     <row r="37" spans="1:4" ht="28" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>48</v>
@@ -1317,7 +1314,7 @@
         <v>48</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
remove 2 tools/standards from curated_standards.xlsx: NuSMV & LoLA; recreate evaluated_standards.tex & evaluated_standards.tsv
</commit_message>
<xml_diff>
--- a/curated_standards.xlsx
+++ b/curated_standards.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32260" yWindow="2040" windowWidth="23820" windowHeight="19560" tabRatio="352"/>
+    <workbookView xWindow="-21100" yWindow="640" windowWidth="21020" windowHeight="20840" tabRatio="352"/>
   </bookViews>
   <sheets>
     <sheet name="Curated_standards" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
   <si>
     <t>Standard / tool</t>
   </si>
@@ -38,15 +38,9 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Pathway Tools</t>
   </si>
   <si>
-    <t>new citation</t>
-  </si>
-  <si>
     <t>SBML</t>
   </si>
   <si>
@@ -263,9 +257,6 @@
     <t>BpForms and BcForms: Tools for concretely describing non-canonical polymers and complexes to facilitate comprehensive biochemical networks</t>
   </si>
   <si>
-    <t>in press</t>
-  </si>
-  <si>
     <t>CellML</t>
   </si>
   <si>
@@ -287,15 +278,6 @@
     <t>Kinetic simulation algorithm ontology</t>
   </si>
   <si>
-    <t>couldn't find KiSAO article with citations</t>
-  </si>
-  <si>
-    <t>LoLA</t>
-  </si>
-  <si>
-    <t>LoLA A Low Level Analyser</t>
-  </si>
-  <si>
     <t>Memote</t>
   </si>
   <si>
@@ -303,12 +285,6 @@
   </si>
   <si>
     <t>Memote: A community driven effort towards a standardized genome-scale metabolic model test suite</t>
-  </si>
-  <si>
-    <t>NuSMV</t>
-  </si>
-  <si>
-    <t>NuSMV 2: An OpenSource Tool for Symbolic Model Checking</t>
   </si>
   <si>
     <t>PROV</t>
@@ -427,16 +403,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -809,12 +782,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="1420" activePane="bottomLeft"/>
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -822,11 +795,10 @@
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="65" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5" style="2"/>
+    <col min="4" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -836,524 +808,478 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="30" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
+      <c r="B44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A43" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="28" x14ac:dyDescent="0.15">
-      <c r="A44" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="42" x14ac:dyDescent="0.15">
-      <c r="A45" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bib entries, esp. removing duplicates; regenerate evaluated_standards.*
</commit_message>
<xml_diff>
--- a/curated_standards.xlsx
+++ b/curated_standards.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21100" yWindow="640" windowWidth="21020" windowHeight="20840" tabRatio="352"/>
+    <workbookView xWindow="1800" yWindow="460" windowWidth="31020" windowHeight="20840" tabRatio="352"/>
   </bookViews>
   <sheets>
     <sheet name="Curated_standards" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>Model repository</t>
   </si>
   <si>
-    <t>BioModels Database: An enhanced, curated and annotated resource for published quantitative kinetic models</t>
-  </si>
-  <si>
     <t>BioPAX</t>
   </si>
   <si>
@@ -339,6 +336,9 @@
   </si>
   <si>
     <t>SciPy optimize, ODE solver, etc.</t>
+  </si>
+  <si>
+    <t>BioModels Database: an enhanced, curated and annotated resource for published quantitative kinetic models</t>
   </si>
 </sst>
 </file>
@@ -787,14 +787,14 @@
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="1420" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="65" style="1" customWidth="1"/>
+    <col min="3" max="3" width="73" style="1" customWidth="1"/>
     <col min="4" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
@@ -820,15 +820,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -839,73 +839,73 @@
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
@@ -919,59 +919,59 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
@@ -987,46 +987,46 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1034,10 +1034,10 @@
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1045,65 +1045,65 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1111,13 +1111,13 @@
         <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1128,12 +1128,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>10</v>
@@ -1141,13 +1141,13 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1155,7 +1155,7 @@
         <v>21</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>22</v>
@@ -1163,112 +1163,112 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
update curated_standards.xlsx; better handle the table caption; add two entries to guidelines_4_repro_models_2020__curated_standards.bib
</commit_message>
<xml_diff>
--- a/curated_standards.xlsx
+++ b/curated_standards.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="460" windowWidth="31020" windowHeight="20840" tabRatio="352"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25220" windowHeight="15540" tabRatio="352"/>
   </bookViews>
   <sheets>
     <sheet name="Curated_standards" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
   <si>
     <t>Standard / tool</t>
   </si>
@@ -80,12 +80,6 @@
     <t>Virtual Cell modelling and simulation software environment</t>
   </si>
   <si>
-    <t>Antimony</t>
-  </si>
-  <si>
-    <t>Antimony: a modular model definition language</t>
-  </si>
-  <si>
     <t>SBGN</t>
   </si>
   <si>
@@ -339,13 +333,25 @@
   </si>
   <si>
     <t>BioModels Database: an enhanced, curated and annotated resource for published quantitative kinetic models</t>
+  </si>
+  <si>
+    <t>OpenCOR</t>
+  </si>
+  <si>
+    <t>Physiome</t>
+  </si>
+  <si>
+    <t>Integration from proteins to organs: the Physiome Project</t>
+  </si>
+  <si>
+    <t>OpenCOR: a modular and interoperable approach to computational biology</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -378,6 +384,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -403,7 +414,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -412,6 +423,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -782,12 +794,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1420" activePane="bottomLeft"/>
+      <pane ySplit="1420" topLeftCell="A28" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -809,67 +821,67 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>74</v>
@@ -877,21 +889,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>41</v>
@@ -899,387 +911,398 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="1" t="s">
-        <v>15</v>
+      <c r="A44" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>16</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Object tables (ObjTables)
</commit_message>
<xml_diff>
--- a/curated_standards.xlsx
+++ b/curated_standards.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25220" windowHeight="15540" tabRatio="352"/>
+    <workbookView xWindow="4040" yWindow="460" windowWidth="25220" windowHeight="18500" tabRatio="352"/>
   </bookViews>
   <sheets>
     <sheet name="Curated_standards" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
   <si>
     <t>Standard / tool</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>OpenCOR: a modular and interoperable approach to computational biology</t>
+  </si>
+  <si>
+    <t>ObjTables</t>
+  </si>
+  <si>
+    <t>Structured spreadsheets with ObjTables enable data reuse and integration</t>
   </si>
 </sst>
 </file>
@@ -794,12 +800,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1420" topLeftCell="A28" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1320" topLeftCell="A28" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1305,6 +1311,17 @@
         <v>104</v>
       </c>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
fix citation error detected by Cell Systems editors
</commit_message>
<xml_diff>
--- a/curated_standards.xlsx
+++ b/curated_standards.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
   <si>
     <t>Standard / tool</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>KiSAO</t>
-  </si>
-  <si>
-    <t>Kinetic simulation algorithm ontology</t>
   </si>
   <si>
     <t>Memote</t>
@@ -803,9 +800,9 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="1320" topLeftCell="A28" activePane="bottomLeft"/>
+      <pane ySplit="1320" topLeftCell="A9" activePane="bottomLeft"/>
       <selection activeCell="D1" sqref="D1:D1048576"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -832,7 +829,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>70</v>
@@ -846,7 +843,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -865,7 +862,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
@@ -931,7 +928,7 @@
         <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>48</v>
@@ -942,7 +939,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>52</v>
@@ -975,7 +972,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>46</v>
@@ -1000,7 +997,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
@@ -1016,13 +1013,13 @@
     </row>
     <row r="19" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1030,7 +1027,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>27</v>
@@ -1041,10 +1038,10 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1052,21 +1049,21 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
@@ -1074,7 +1071,7 @@
         <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>67</v>
@@ -1085,7 +1082,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>62</v>
@@ -1107,7 +1104,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>29</v>
@@ -1118,7 +1115,7 @@
         <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -1140,7 +1137,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>10</v>
@@ -1162,7 +1159,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>20</v>
@@ -1181,7 +1178,7 @@
     </row>
     <row r="34" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>43</v>
@@ -1192,13 +1189,13 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1225,13 +1222,13 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1242,7 +1239,7 @@
         <v>34</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1253,7 +1250,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="28" x14ac:dyDescent="0.15">
@@ -1291,35 +1288,35 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>